<commit_message>
DATA: include VE estimates for doses 1-5 against wildtype
</commit_message>
<xml_diff>
--- a/inst/extdata/inputs/ve_dat.xlsx
+++ b/inst/extdata/inputs/ve_dat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\R\ainsliek\code\vacamole\inst\extdata\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4ED6DBC7-DCB1-456D-9A6A-2D1108D2919F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{911CEC35-F817-478C-8AC2-CC39410272C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="240" windowWidth="11085" windowHeight="15165" xr2:uid="{E62D7B7E-56A5-4CC4-8D62-76C0596AA6AC}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H438" sqref="H438"/>
     </sheetView>
   </sheetViews>

</xml_diff>